<commit_message>
Erster Stand Belaria R290 60 kW mit H (Heizen) und C (kühlen) Noch ohne IHX INPUT: input//HPSetpoints.xlsx  & input//CHSetpoints.xlsx OUTPUT: output//HPResult.xlsx & Chiller_Result.xlsx
Belariapro65H_SH5 = Belariapro65H(VZN175, B250ASHx90, LuftKM_OEMWT.Sierra_2519_BelPro60_SH5, noiwt, B220Hx128,
                                  ZA_FP063_4)
Belariapro65C_SH5 = Belariapro65C(VZN175, LuftKM_OEMWT.Sierra_2519_BelPro60_Cond, F250ASHx90, noiwt, B220Hx128,
                                  ZA_FP063_4)
Fehler im IHX gefunden und korrigiert.
</commit_message>
<xml_diff>
--- a/INPUT/CHSetpoints.xlsx
+++ b/INPUT/CHSetpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WP Jumbo\INPUT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E87CCFC-DF95-4493-905C-15450398EDA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3153D821-EBCB-4CD1-83AE-585E9CB7EAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39870" yWindow="2530" windowWidth="35250" windowHeight="15460" xr2:uid="{A6AE4BAC-2A93-431D-9AF1-84B4A36349B0}"/>
+    <workbookView xWindow="6010" yWindow="1330" windowWidth="35250" windowHeight="15450" xr2:uid="{A6AE4BAC-2A93-431D-9AF1-84B4A36349B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -402,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6DF9AC-AC96-4E81-92BF-929A0FD33CFA}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -473,12 +473,12 @@
         <v>140</v>
       </c>
       <c r="F3">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>42</v>
@@ -493,12 +493,12 @@
         <v>140</v>
       </c>
       <c r="F4">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>42</v>
@@ -513,7 +513,7 @@
         <v>140</v>
       </c>
       <c r="F5">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -521,7 +521,7 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -530,10 +530,10 @@
         <v>24000</v>
       </c>
       <c r="E6">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="F6">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -541,7 +541,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -550,18 +550,18 @@
         <v>24000</v>
       </c>
       <c r="E7">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="F7">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -570,10 +570,10 @@
         <v>24000</v>
       </c>
       <c r="E8">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="F8">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -581,7 +581,7 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -590,10 +590,430 @@
         <v>24000</v>
       </c>
       <c r="E9">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="F9">
         <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>42</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>24000</v>
+      </c>
+      <c r="E10">
+        <v>140</v>
+      </c>
+      <c r="F10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>24000</v>
+      </c>
+      <c r="E11">
+        <v>120</v>
+      </c>
+      <c r="F11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>32</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>24000</v>
+      </c>
+      <c r="E12">
+        <v>120</v>
+      </c>
+      <c r="F12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>24000</v>
+      </c>
+      <c r="E13">
+        <v>120</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>32</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>24000</v>
+      </c>
+      <c r="E14">
+        <v>120</v>
+      </c>
+      <c r="F14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>28000</v>
+      </c>
+      <c r="E15">
+        <v>140</v>
+      </c>
+      <c r="F15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>35</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>28000</v>
+      </c>
+      <c r="E16">
+        <v>140</v>
+      </c>
+      <c r="F16">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>30</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>28000</v>
+      </c>
+      <c r="E17">
+        <v>140</v>
+      </c>
+      <c r="F17">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>28000</v>
+      </c>
+      <c r="E18">
+        <v>140</v>
+      </c>
+      <c r="F18">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <v>40</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>28000</v>
+      </c>
+      <c r="E19">
+        <v>140</v>
+      </c>
+      <c r="F19">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20">
+        <v>35</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>28000</v>
+      </c>
+      <c r="E20">
+        <v>140</v>
+      </c>
+      <c r="F20">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>14</v>
+      </c>
+      <c r="B21">
+        <v>30</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>28000</v>
+      </c>
+      <c r="E21">
+        <v>140</v>
+      </c>
+      <c r="F21">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>14</v>
+      </c>
+      <c r="B22">
+        <v>25</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>28000</v>
+      </c>
+      <c r="E22">
+        <v>140</v>
+      </c>
+      <c r="F22">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>40</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>28000</v>
+      </c>
+      <c r="E23">
+        <v>100</v>
+      </c>
+      <c r="F23">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>35</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>28000</v>
+      </c>
+      <c r="E24">
+        <v>100</v>
+      </c>
+      <c r="F24">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <v>30</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>28000</v>
+      </c>
+      <c r="E25">
+        <v>100</v>
+      </c>
+      <c r="F25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <v>28000</v>
+      </c>
+      <c r="E26">
+        <v>100</v>
+      </c>
+      <c r="F26">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>40</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>20000</v>
+      </c>
+      <c r="E27">
+        <v>90</v>
+      </c>
+      <c r="F27">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>14</v>
+      </c>
+      <c r="B28">
+        <v>35</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>20000</v>
+      </c>
+      <c r="E28">
+        <v>90</v>
+      </c>
+      <c r="F28">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>30</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>20000</v>
+      </c>
+      <c r="E29">
+        <v>90</v>
+      </c>
+      <c r="F29">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>14</v>
+      </c>
+      <c r="B30">
+        <v>25</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>20000</v>
+      </c>
+      <c r="E30">
+        <v>90</v>
+      </c>
+      <c r="F30">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>